<commit_message>
color and protection code
</commit_message>
<xml_diff>
--- a/tests/spectrum_etl/edc/single_cell_suspension.xlsx
+++ b/tests/spectrum_etl/edc/single_cell_suspension.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-33820" yWindow="3760" windowWidth="25760" windowHeight="13880" tabRatio="500"/>
+    <workbookView xWindow="-35780" yWindow="1680" windowWidth="31200" windowHeight="20360" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NOTES" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
   <si>
     <t>patient_mrn</t>
   </si>
@@ -193,6 +193,24 @@
   </si>
   <si>
     <t xml:space="preserve">4. Follow the usage pattern above to add new values with the changes needed </t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>specimen_id_fk</t>
+  </si>
+  <si>
+    <t>add notes for hacking the sheet</t>
+  </si>
+  <si>
+    <t>add a field to show row is locked</t>
   </si>
 </sst>
 </file>
@@ -239,7 +257,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,6 +282,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -281,17 +305,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -573,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -816,6 +844,16 @@
         <v>53</v>
       </c>
     </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C38" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C39" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -825,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -845,14 +883,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
-        <v>1234567</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>12345</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -860,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -882,22 +921,22 @@
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
+      <c r="A2" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="AA2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="AA3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="AA4" t="s">
         <v>7</v>
       </c>
@@ -915,10 +954,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -928,7 +967,7 @@
     <col min="3" max="3" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -937,6 +976,81 @@
       </c>
       <c r="C1" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>5</v>
+      </c>
+      <c r="B5" s="8">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>7</v>
+      </c>
+      <c r="B7" s="8">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -946,20 +1060,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA9"/>
+  <dimension ref="A1:AB9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="10.83203125" style="3"/>
+    <col min="5" max="5" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -973,56 +1088,65 @@
         <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="AA2" t="s">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="F2" s="3">
+        <v>11</v>
+      </c>
+      <c r="AB2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="AA3" t="s">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="F3" s="3">
+        <v>12</v>
+      </c>
+      <c r="AB3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="AA4" t="s">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="AA5" t="s">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="AA6" t="s">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="AA7" t="s">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="AA8" t="s">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="AA9" t="s">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AB9" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A302">
-      <formula1>$AA$2:$AA$9</formula1>
+      <formula1>$AB$2:$AB$9</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>